<commit_message>
11 & 12 & 13
</commit_message>
<xml_diff>
--- a/file/2008年德阳市国民经济和社会发展统计公报.xlsx
+++ b/file/2008年德阳市国民经济和社会发展统计公报.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="157">
   <si>
     <t>人口</t>
   </si>
@@ -430,12 +430,6 @@
   </si>
   <si>
     <t>7560公里</t>
-  </si>
-  <si>
-    <t>13.7亿吨公里</t>
-  </si>
-  <si>
-    <t>14.6亿人公里</t>
   </si>
   <si>
     <t>42.9亿元</t>
@@ -1168,7 +1162,7 @@
         <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4">
@@ -1176,7 +1170,7 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
@@ -1200,10 +1194,10 @@
         <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12">
@@ -1222,10 +1216,10 @@
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1246,10 +1240,10 @@
         <v>63</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
@@ -1257,10 +1251,10 @@
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
@@ -1268,10 +1262,10 @@
         <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12">
@@ -1279,7 +1273,7 @@
         <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D12" t="s">
         <v>79</v>
@@ -1334,13 +1328,13 @@
         <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8">
@@ -1348,13 +1342,13 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
         <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9">
@@ -1362,13 +1356,13 @@
         <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
         <v>79</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10">
@@ -1376,13 +1370,13 @@
         <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C10" t="s">
         <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11">
@@ -1390,13 +1384,13 @@
         <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
         <v>79</v>
       </c>
       <c r="D11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>